<commit_message>
some results and more classified words
</commit_message>
<xml_diff>
--- a/animals words.xlsx
+++ b/animals words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AVI\PycharmProjects\useGensim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B652DB-EDE9-44FD-9D79-A03266A706F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901528BC-1AB9-42C4-AC8A-09B2873D2E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words list" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="3273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="3457">
   <si>
     <t>Aardvark</t>
   </si>
@@ -9854,13 +9854,565 @@
   </si>
   <si>
     <t>Yorkshire_terrier</t>
+  </si>
+  <si>
+    <t>Bobolink</t>
+  </si>
+  <si>
+    <t>Cats_Meow</t>
+  </si>
+  <si>
+    <t>S_Zervan</t>
+  </si>
+  <si>
+    <t>Pinup_Girl</t>
+  </si>
+  <si>
+    <t>Trippers</t>
+  </si>
+  <si>
+    <t>Egret</t>
+  </si>
+  <si>
+    <t>Sippers</t>
+  </si>
+  <si>
+    <t>Ringmasters</t>
+  </si>
+  <si>
+    <t>Mynah</t>
+  </si>
+  <si>
+    <t>Dollz</t>
+  </si>
+  <si>
+    <t>Pearly_Whites</t>
+  </si>
+  <si>
+    <t>Tamers</t>
+  </si>
+  <si>
+    <t>Wampus</t>
+  </si>
+  <si>
+    <t>Rock'N'Roll</t>
+  </si>
+  <si>
+    <t>Woodys</t>
+  </si>
+  <si>
+    <t>Yah_Yah</t>
+  </si>
+  <si>
+    <t>Lucky</t>
+  </si>
+  <si>
+    <t>Jewelled</t>
+  </si>
+  <si>
+    <t>Gruv</t>
+  </si>
+  <si>
+    <t>Double_crested_Cormorant</t>
+  </si>
+  <si>
+    <t>Cool_Breeze</t>
+  </si>
+  <si>
+    <t>Captive_bred</t>
+  </si>
+  <si>
+    <t>Brokedown</t>
+  </si>
+  <si>
+    <t>Cotley</t>
+  </si>
+  <si>
+    <t>Whale_Spotted</t>
+  </si>
+  <si>
+    <t>Swingset</t>
+  </si>
+  <si>
+    <t>Willies</t>
+  </si>
+  <si>
+    <t>Lucky_Leprechaun</t>
+  </si>
+  <si>
+    <t>Wubbzy</t>
+  </si>
+  <si>
+    <t>Silverfish</t>
+  </si>
+  <si>
+    <t>Zany</t>
+  </si>
+  <si>
+    <t>Yabba_Dabba_Doo</t>
+  </si>
+  <si>
+    <t>Droids_Attack</t>
+  </si>
+  <si>
+    <t>Slink</t>
+  </si>
+  <si>
+    <t>CASINO_NIAGARA</t>
+  </si>
+  <si>
+    <t>dart_frogs</t>
+  </si>
+  <si>
+    <t>Schlong</t>
+  </si>
+  <si>
+    <t>Bushtucker</t>
+  </si>
+  <si>
+    <t>Evenflo_Recalls</t>
+  </si>
+  <si>
+    <t>Jabroni</t>
+  </si>
+  <si>
+    <t>Punx</t>
+  </si>
+  <si>
+    <t>Pint_Sized</t>
+  </si>
+  <si>
+    <t>Arowana</t>
+  </si>
+  <si>
+    <t>Wallies</t>
+  </si>
+  <si>
+    <t>Fanci</t>
+  </si>
+  <si>
+    <t>Stranded_Whales</t>
+  </si>
+  <si>
+    <t>Bubblegum</t>
+  </si>
+  <si>
+    <t>Fishies</t>
+  </si>
+  <si>
+    <t>Geezer</t>
+  </si>
+  <si>
+    <t>Oarsman</t>
+  </si>
+  <si>
+    <t>Lochlin</t>
+  </si>
+  <si>
+    <t>Butterfish</t>
+  </si>
+  <si>
+    <t>Snip_Snip</t>
+  </si>
+  <si>
+    <t>Puss_Puss</t>
+  </si>
+  <si>
+    <t>Buteo</t>
+  </si>
+  <si>
+    <t>Frugal_Fun</t>
+  </si>
+  <si>
+    <t>Crackhouse</t>
+  </si>
+  <si>
+    <t>Outerspace</t>
+  </si>
+  <si>
+    <t>Salmonella_Outbreak_Linked</t>
+  </si>
+  <si>
+    <t>Birds</t>
+  </si>
+  <si>
+    <t>Daylight_Robbery</t>
+  </si>
+  <si>
+    <t>Red_Legged_Frog</t>
+  </si>
+  <si>
+    <t>Flesh_Eating_Bacteria</t>
+  </si>
+  <si>
+    <t>Lemur_Island</t>
+  </si>
+  <si>
+    <t>&amp;_Claws_Pet</t>
+  </si>
+  <si>
+    <t>Frog_Legs</t>
+  </si>
+  <si>
+    <t>Pufnstuf</t>
+  </si>
+  <si>
+    <t>Hoo_Ha</t>
+  </si>
+  <si>
+    <t>Corpse_Found</t>
+  </si>
+  <si>
+    <t>Shortcake</t>
+  </si>
+  <si>
+    <t>Wog</t>
+  </si>
+  <si>
+    <t>Frozen_Margarita</t>
+  </si>
+  <si>
+    <t>Flamers</t>
+  </si>
+  <si>
+    <t>camels_zebras</t>
+  </si>
+  <si>
+    <t>Pterosaur</t>
+  </si>
+  <si>
+    <t>Robber_Holds_Up</t>
+  </si>
+  <si>
+    <t>Ants</t>
+  </si>
+  <si>
+    <t>Hunter_Gatherer</t>
+  </si>
+  <si>
+    <t>Pedal_Paddle</t>
+  </si>
+  <si>
+    <t>Giant_Squid</t>
+  </si>
+  <si>
+    <t>Twig</t>
+  </si>
+  <si>
+    <t>Blooze</t>
+  </si>
+  <si>
+    <t>Girl</t>
+  </si>
+  <si>
+    <t>Repellant</t>
+  </si>
+  <si>
+    <t>Silkie</t>
+  </si>
+  <si>
+    <t>Eastern_Screech_Owl</t>
+  </si>
+  <si>
+    <t>Laughing_Gravy</t>
+  </si>
+  <si>
+    <t>Fadeaway</t>
+  </si>
+  <si>
+    <t>WowWee_Alive</t>
+  </si>
+  <si>
+    <t>Couch_Potatoes</t>
+  </si>
+  <si>
+    <t>Puddin</t>
+  </si>
+  <si>
+    <t>Porta_Puppet_Players</t>
+  </si>
+  <si>
+    <t>Another_Roadside_Attraction</t>
+  </si>
+  <si>
+    <t>Dromedary</t>
+  </si>
+  <si>
+    <t>SUV_Slams_Into</t>
+  </si>
+  <si>
+    <t>Sk8er</t>
+  </si>
+  <si>
+    <t>Rootbeer</t>
+  </si>
+  <si>
+    <t>Zedonk</t>
+  </si>
+  <si>
+    <t>Wolfies</t>
+  </si>
+  <si>
+    <t>Orchid</t>
+  </si>
+  <si>
+    <t>Molehill</t>
+  </si>
+  <si>
+    <t>Bawl</t>
+  </si>
+  <si>
+    <t>Has_Landed</t>
+  </si>
+  <si>
+    <t>Flapjack</t>
+  </si>
+  <si>
+    <t>Justine_Blazer</t>
+  </si>
+  <si>
+    <t>Oggy</t>
+  </si>
+  <si>
+    <t>Code_Geass</t>
+  </si>
+  <si>
+    <t>Poopsie</t>
+  </si>
+  <si>
+    <t>Yardsale</t>
+  </si>
+  <si>
+    <t>Stoplight</t>
+  </si>
+  <si>
+    <t>Grrls</t>
+  </si>
+  <si>
+    <t>Old_Farts</t>
+  </si>
+  <si>
+    <t>Heavier_Than</t>
+  </si>
+  <si>
+    <t>Silly_Songs</t>
+  </si>
+  <si>
+    <t>Kabocha_Squash</t>
+  </si>
+  <si>
+    <t>Sumpin</t>
+  </si>
+  <si>
+    <t>Pumpkinhead</t>
+  </si>
+  <si>
+    <t>Julie_Garwood_Ballantine</t>
+  </si>
+  <si>
+    <t>Beater</t>
+  </si>
+  <si>
+    <t>Poochie</t>
+  </si>
+  <si>
+    <t>Crash_Victim_Dies</t>
+  </si>
+  <si>
+    <t>Ugliest_Dog</t>
+  </si>
+  <si>
+    <t>Patter</t>
+  </si>
+  <si>
+    <t>Wat_er</t>
+  </si>
+  <si>
+    <t>Blueberry_Pancakes</t>
+  </si>
+  <si>
+    <t>Loses_Arm</t>
+  </si>
+  <si>
+    <t>OX4</t>
+  </si>
+  <si>
+    <t>Gun_Wielding</t>
+  </si>
+  <si>
+    <t>Bikini_Babes</t>
+  </si>
+  <si>
+    <t>Steller_Sea</t>
+  </si>
+  <si>
+    <t>sun_conures</t>
+  </si>
+  <si>
+    <t>Walmart_Parking_Lot</t>
+  </si>
+  <si>
+    <t>Loosen_Up</t>
+  </si>
+  <si>
+    <t>Light_###.#p_###.#p</t>
+  </si>
+  <si>
+    <t>Spinnerbait</t>
+  </si>
+  <si>
+    <t>Burlesque_Revue</t>
+  </si>
+  <si>
+    <t>Ugly_Bug</t>
+  </si>
+  <si>
+    <t>DJ_Icey</t>
+  </si>
+  <si>
+    <t>Spoonbills</t>
+  </si>
+  <si>
+    <t>Flower_Pot</t>
+  </si>
+  <si>
+    <t>Pet_Look_Alike</t>
+  </si>
+  <si>
+    <t>Scotty_Karate</t>
+  </si>
+  <si>
+    <t>Bait_Shack</t>
+  </si>
+  <si>
+    <t>Foot_Python</t>
+  </si>
+  <si>
+    <t>Humpback_Whales</t>
+  </si>
+  <si>
+    <t>Icey</t>
+  </si>
+  <si>
+    <t>Dumplin</t>
+  </si>
+  <si>
+    <t>Beehives</t>
+  </si>
+  <si>
+    <t>Lollies</t>
+  </si>
+  <si>
+    <t>Muncher</t>
+  </si>
+  <si>
+    <t>WORLD_CAFÉ_LIVE</t>
+  </si>
+  <si>
+    <t>Goldminer</t>
+  </si>
+  <si>
+    <t>Shags</t>
+  </si>
+  <si>
+    <t>Shrinking_Violets</t>
+  </si>
+  <si>
+    <t>Duck_Duck</t>
+  </si>
+  <si>
+    <t>Beached_Whale</t>
+  </si>
+  <si>
+    <t>Miniature_Dachshund</t>
+  </si>
+  <si>
+    <t>Hollywild</t>
+  </si>
+  <si>
+    <t>Outwits</t>
+  </si>
+  <si>
+    <t>Jurrasic</t>
+  </si>
+  <si>
+    <t>Skanky</t>
+  </si>
+  <si>
+    <t>Araucana</t>
+  </si>
+  <si>
+    <t>Flat_Tire</t>
+  </si>
+  <si>
+    <t>BCN_Healthy</t>
+  </si>
+  <si>
+    <t>fin_tuna</t>
+  </si>
+  <si>
+    <t>Aunti</t>
+  </si>
+  <si>
+    <t>Darkling</t>
+  </si>
+  <si>
+    <t>Worrier</t>
+  </si>
+  <si>
+    <t>extinct_Tasmanian</t>
+  </si>
+  <si>
+    <t>Spittin</t>
+  </si>
+  <si>
+    <t>Fairie</t>
+  </si>
+  <si>
+    <t>Churro</t>
+  </si>
+  <si>
+    <t>Potato_Pie</t>
+  </si>
+  <si>
+    <t>Mollies</t>
+  </si>
+  <si>
+    <t>Saber_Toothed_Tiger</t>
+  </si>
+  <si>
+    <t>Tiny_Tears</t>
+  </si>
+  <si>
+    <t>Licorice</t>
+  </si>
+  <si>
+    <t>TIGHT_LINES</t>
+  </si>
+  <si>
+    <t>Hawksbill_Turtle</t>
+  </si>
+  <si>
+    <t>Turtles</t>
+  </si>
+  <si>
+    <t>Too_Far_Away</t>
+  </si>
+  <si>
+    <t>BOOK_REVIEWS</t>
+  </si>
+  <si>
+    <t>Guns_Ammo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B_**_ch </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10032,6 +10584,18 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -10381,7 +10945,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -10400,6 +10964,10 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -10725,10 +11293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AC216F-559C-4988-B135-E2C7D7D78959}">
-  <dimension ref="A1:A1657"/>
+  <dimension ref="A1:A1684"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1658" sqref="B1658"/>
+    <sheetView rightToLeft="1" topLeftCell="A1653" workbookViewId="0">
+      <selection activeCell="A1684" sqref="A1684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10851,7 +11419,7 @@
         <v>2482</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="28.5">
+    <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
         <v>340</v>
       </c>
@@ -19019,6 +19587,141 @@
     <row r="1657" spans="1:1">
       <c r="A1657" s="6" t="s">
         <v>3170</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:1">
+      <c r="A1658" s="4" t="s">
+        <v>3273</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:1" ht="15">
+      <c r="A1659" s="8" t="s">
+        <v>3278</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:1" ht="15">
+      <c r="A1660" s="8" t="s">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:1" ht="15">
+      <c r="A1661" s="8" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:1" ht="15">
+      <c r="A1662" s="8" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:1" ht="15">
+      <c r="A1663" s="8" t="s">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:1" ht="15">
+      <c r="A1664" s="8" t="s">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:1" ht="15">
+      <c r="A1665" s="8" t="s">
+        <v>3324</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:1" ht="15">
+      <c r="A1666" s="8" t="s">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:1" ht="15">
+      <c r="A1667" s="8" t="s">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:1" ht="15">
+      <c r="A1668" s="8" t="s">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:1" ht="15">
+      <c r="A1669" s="8" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:1" ht="15">
+      <c r="A1670" s="8" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:1" ht="15">
+      <c r="A1671" s="8" t="s">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:1" ht="15">
+      <c r="A1672" s="8" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:1" ht="15">
+      <c r="A1673" s="8" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:1" ht="15">
+      <c r="A1674" s="8" t="s">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:1" ht="15">
+      <c r="A1675" s="8" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:1" ht="15">
+      <c r="A1676" s="8" t="s">
+        <v>3411</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:1" ht="15">
+      <c r="A1677" s="8" t="s">
+        <v>3417</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:1" ht="15">
+      <c r="A1678" s="8" t="s">
+        <v>3425</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:1" ht="15">
+      <c r="A1679" s="8" t="s">
+        <v>3429</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:1" ht="15">
+      <c r="A1680" s="8" t="s">
+        <v>3434</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:1" ht="15">
+      <c r="A1681" s="8" t="s">
+        <v>3447</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:1" ht="15">
+      <c r="A1682" s="8" t="s">
+        <v>3446</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:1" ht="15">
+      <c r="A1683" s="7" t="s">
+        <v>3451</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:1" ht="15">
+      <c r="A1684" s="7" t="s">
+        <v>3452</v>
       </c>
     </row>
   </sheetData>
@@ -19032,10 +19735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BCBB88-EB20-4FE9-9853-5AEACCACF1D8}">
-  <dimension ref="A1:B1623"/>
+  <dimension ref="A1:B1780"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A1598" workbookViewId="0">
-      <selection activeCell="A1598" sqref="A1:A1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A1774" workbookViewId="0">
+      <selection activeCell="A1780" sqref="A1780"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -27185,6 +27888,791 @@
         <v>2474</v>
       </c>
     </row>
+    <row r="1624" spans="1:1" ht="15">
+      <c r="A1624" s="7" t="s">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:1" ht="15">
+      <c r="A1625" s="7" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:1" ht="15">
+      <c r="A1626" s="8" t="s">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:1" ht="15">
+      <c r="A1627" s="8" t="s">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:1" ht="15">
+      <c r="A1628" s="8" t="s">
+        <v>3279</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:1" ht="15">
+      <c r="A1629" s="8" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:1" ht="15">
+      <c r="A1630" s="8" t="s">
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:1" ht="15">
+      <c r="A1631" s="8" t="s">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:1" ht="15">
+      <c r="A1632" s="8" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:1" ht="15">
+      <c r="A1633" s="8" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:1" ht="15">
+      <c r="A1634" s="8" t="s">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:1" ht="15">
+      <c r="A1635" s="8" t="s">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:1" ht="15">
+      <c r="A1636" s="8" t="s">
+        <v>3288</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:1" ht="15">
+      <c r="A1637" s="8" t="s">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:1" ht="15">
+      <c r="A1638" s="8" t="s">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:1" ht="15">
+      <c r="A1639" s="8" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:1" ht="15">
+      <c r="A1640" s="8" t="s">
+        <v>3293</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:1" ht="15">
+      <c r="A1641" s="8" t="s">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:1" ht="15">
+      <c r="A1642" s="8" t="s">
+        <v>3295</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:1" ht="15">
+      <c r="A1643" s="8" t="s">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:1" ht="15">
+      <c r="A1644" s="8" t="s">
+        <v>3297</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:1" ht="15">
+      <c r="A1645" s="8" t="s">
+        <v>3298</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:1" ht="15">
+      <c r="A1646" s="8" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:1" ht="15">
+      <c r="A1647" s="8" t="s">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:1" ht="15">
+      <c r="A1648" s="8" t="s">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:1" ht="15">
+      <c r="A1649" s="8" t="s">
+        <v>3303</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:1" ht="15">
+      <c r="A1650" s="8" t="s">
+        <v>3304</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:1" ht="15">
+      <c r="A1651" s="8" t="s">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:1" ht="15">
+      <c r="A1652" s="8" t="s">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:1" ht="15">
+      <c r="A1653" s="8" t="s">
+        <v>3307</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:1" ht="15">
+      <c r="A1654" s="8" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:1" ht="15">
+      <c r="A1655" s="8" t="s">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:1" ht="15">
+      <c r="A1656" s="8" t="s">
+        <v>3311</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:1" ht="15">
+      <c r="A1657" s="8" t="s">
+        <v>3312</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:1" ht="15">
+      <c r="A1658" s="8" t="s">
+        <v>3313</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:1" ht="15">
+      <c r="A1659" s="8" t="s">
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:1" ht="15">
+      <c r="A1660" s="8" t="s">
+        <v>3316</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:1" ht="15">
+      <c r="A1661" s="8" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:1" ht="15">
+      <c r="A1662" s="8" t="s">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:1" ht="15">
+      <c r="A1663" s="8" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:1" ht="15">
+      <c r="A1664" s="8" t="s">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:1" ht="15">
+      <c r="A1665" s="8" t="s">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:1" ht="15">
+      <c r="A1666" s="8" t="s">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:1" ht="15">
+      <c r="A1667" s="8" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:1" ht="15">
+      <c r="A1668" s="8" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:1" ht="15">
+      <c r="A1669" s="8" t="s">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:1" ht="15">
+      <c r="A1670" s="8" t="s">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:1" ht="15">
+      <c r="A1671" s="8" t="s">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:1" ht="15">
+      <c r="A1672" s="8" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:1" ht="15">
+      <c r="A1673" s="8" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:1" ht="15">
+      <c r="A1674" s="8" t="s">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:1" ht="15">
+      <c r="A1675" s="8" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:1" ht="15">
+      <c r="A1676" s="8" t="s">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:1" ht="15">
+      <c r="A1677" s="8" t="s">
+        <v>3337</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:1" ht="15">
+      <c r="A1678" s="8" t="s">
+        <v>3338</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:1" ht="15">
+      <c r="A1679" s="8" t="s">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:1" ht="15">
+      <c r="A1680" s="8" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:1" ht="15">
+      <c r="A1681" s="8" t="s">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:1" ht="15">
+      <c r="A1682" s="8" t="s">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:1" ht="15">
+      <c r="A1683" s="8" t="s">
+        <v>3343</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:1" ht="15">
+      <c r="A1684" s="8" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:1" ht="15">
+      <c r="A1685" s="8" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:1" ht="15">
+      <c r="A1686" s="8" t="s">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:1" ht="15">
+      <c r="A1687" s="8" t="s">
+        <v>3348</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:1" ht="15">
+      <c r="A1688" s="8" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:1" ht="15">
+      <c r="A1689" s="8" t="s">
+        <v>3351</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:1" ht="15">
+      <c r="A1690" s="8" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:1" ht="15">
+      <c r="A1691" s="8" t="s">
+        <v>3354</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:1" ht="15">
+      <c r="A1692" s="8" t="s">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:1" ht="15">
+      <c r="A1693" s="8" t="s">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:1" ht="15">
+      <c r="A1694" s="8" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:1" ht="15">
+      <c r="A1695" s="8" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:1" ht="15">
+      <c r="A1696" s="8" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:1" ht="15">
+      <c r="A1697" s="8" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:1" ht="15">
+      <c r="A1698" s="8" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:1" ht="15">
+      <c r="A1699" s="8" t="s">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:1" ht="15">
+      <c r="A1700" s="8" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:1" ht="15">
+      <c r="A1701" s="8" t="s">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:1" ht="15">
+      <c r="A1702" s="8" t="s">
+        <v>3368</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:1" ht="15">
+      <c r="A1703" s="8" t="s">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:1" ht="15">
+      <c r="A1704" s="8" t="s">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:1" ht="15">
+      <c r="A1705" s="8" t="s">
+        <v>3371</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:1" ht="15">
+      <c r="A1706" s="8" t="s">
+        <v>3372</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:1" ht="15">
+      <c r="A1707" s="8" t="s">
+        <v>3373</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:1" ht="15">
+      <c r="A1708" s="8" t="s">
+        <v>3374</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:1" ht="15">
+      <c r="A1709" s="8" t="s">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:1" ht="15">
+      <c r="A1710" s="8" t="s">
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:1" ht="15">
+      <c r="A1711" s="8" t="s">
+        <v>3377</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:1" ht="15">
+      <c r="A1712" s="8" t="s">
+        <v>3378</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:1" ht="15">
+      <c r="A1713" s="8" t="s">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:1" ht="15">
+      <c r="A1714" s="8" t="s">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:1" ht="15">
+      <c r="A1715" s="8" t="s">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:1" ht="15">
+      <c r="A1716" s="8" t="s">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:1" ht="15">
+      <c r="A1717" s="8" t="s">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:1" ht="15">
+      <c r="A1718" s="8" t="s">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:1" ht="15">
+      <c r="A1719" s="8" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:1" ht="15">
+      <c r="A1720" s="8" t="s">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:1" ht="15">
+      <c r="A1721" s="8" t="s">
+        <v>3387</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:1" ht="15">
+      <c r="A1722" s="8" t="s">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:1" ht="15">
+      <c r="A1723" s="8" t="s">
+        <v>3389</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:1" ht="15">
+      <c r="A1724" s="8" t="s">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:1" ht="15">
+      <c r="A1725" s="8" t="s">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:1" ht="15">
+      <c r="A1726" s="8" t="s">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:1" ht="15">
+      <c r="A1727" s="8" t="s">
+        <v>3393</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:1" ht="15">
+      <c r="A1728" s="8" t="s">
+        <v>3394</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:1" ht="15">
+      <c r="A1729" s="8" t="s">
+        <v>3395</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:1" ht="15">
+      <c r="A1730" s="8" t="s">
+        <v>3396</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:1" ht="15">
+      <c r="A1731" s="8" t="s">
+        <v>3397</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:1" ht="15">
+      <c r="A1732" s="8" t="s">
+        <v>3398</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:1" ht="15">
+      <c r="A1733" s="8" t="s">
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:1" ht="15">
+      <c r="A1734" s="8" t="s">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:1" ht="15">
+      <c r="A1735" s="8" t="s">
+        <v>3401</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:1" ht="15">
+      <c r="A1736" s="8" t="s">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:1" ht="15">
+      <c r="A1737" s="8" t="s">
+        <v>3404</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:1" ht="15">
+      <c r="A1738" s="8" t="s">
+        <v>3405</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:1" ht="15">
+      <c r="A1739" s="8" t="s">
+        <v>3406</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:1" ht="15">
+      <c r="A1740" s="8" t="s">
+        <v>3407</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:1" ht="15">
+      <c r="A1741" s="8" t="s">
+        <v>3408</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:1" ht="15">
+      <c r="A1742" s="8" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:1" ht="15">
+      <c r="A1743" s="8" t="s">
+        <v>3410</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:1" ht="15">
+      <c r="A1744" s="8" t="s">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:1" ht="15">
+      <c r="A1745" s="8" t="s">
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:1" ht="15">
+      <c r="A1746" s="8" t="s">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:1" ht="15">
+      <c r="A1747" s="8" t="s">
+        <v>3415</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:1" ht="15">
+      <c r="A1748" s="8" t="s">
+        <v>3416</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:1" ht="15">
+      <c r="A1749" s="8" t="s">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:1" ht="15">
+      <c r="A1750" s="8" t="s">
+        <v>3419</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:1" ht="15">
+      <c r="A1751" s="8" t="s">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:1" ht="15">
+      <c r="A1752" s="8" t="s">
+        <v>3421</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:1" ht="15">
+      <c r="A1753" s="8" t="s">
+        <v>3422</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:1" ht="15">
+      <c r="A1754" s="8" t="s">
+        <v>3423</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:1" ht="15">
+      <c r="A1755" s="8" t="s">
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:1" ht="15">
+      <c r="A1756" s="8" t="s">
+        <v>3427</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:1" ht="15">
+      <c r="A1757" s="8" t="s">
+        <v>3426</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:1" ht="15">
+      <c r="A1758" s="8" t="s">
+        <v>3428</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:1" ht="15">
+      <c r="A1759" s="8" t="s">
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:1" ht="15">
+      <c r="A1760" s="8" t="s">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:1" ht="15">
+      <c r="A1761" s="8" t="s">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:1" ht="15">
+      <c r="A1762" s="8" t="s">
+        <v>3433</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:1" ht="15">
+      <c r="A1763" s="8" t="s">
+        <v>3435</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:1" ht="15">
+      <c r="A1764" s="8" t="s">
+        <v>3436</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:1" ht="15">
+      <c r="A1765" s="8" t="s">
+        <v>3437</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:1" ht="15">
+      <c r="A1766" s="8" t="s">
+        <v>3438</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:1" ht="15">
+      <c r="A1767" s="8" t="s">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:1" ht="15">
+      <c r="A1768" s="8" t="s">
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:1" ht="15">
+      <c r="A1769" s="8" t="s">
+        <v>3441</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:1" ht="15">
+      <c r="A1770" s="8" t="s">
+        <v>3442</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:1" ht="15">
+      <c r="A1771" s="8" t="s">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:1" ht="15">
+      <c r="A1772" s="8" t="s">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:1" ht="15">
+      <c r="A1773" s="8" t="s">
+        <v>3445</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:1" ht="15">
+      <c r="A1774" s="8" t="s">
+        <v>3448</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:1" ht="15">
+      <c r="A1775" s="8" t="s">
+        <v>3449</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:1" ht="15">
+      <c r="A1776" s="8" t="s">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:1" ht="15">
+      <c r="A1777" s="7" t="s">
+        <v>3453</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:1" ht="15">
+      <c r="A1778" s="7" t="s">
+        <v>3454</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:1" ht="15">
+      <c r="A1779" s="7" t="s">
+        <v>3455</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:1" ht="15">
+      <c r="A1780" s="7" t="s">
+        <v>3456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update utils and update results
</commit_message>
<xml_diff>
--- a/animals words.xlsx
+++ b/animals words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AVI\PycharmProjects\useGensim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901528BC-1AB9-42C4-AC8A-09B2873D2E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F46E47-537E-41E5-AC72-DCD5A4F42529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words list" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="3457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="3476">
   <si>
     <t>Aardvark</t>
   </si>
@@ -10406,6 +10406,63 @@
   </si>
   <si>
     <t xml:space="preserve">B_**_ch </t>
+  </si>
+  <si>
+    <t>Critter_Care</t>
+  </si>
+  <si>
+    <t>Cotton_Tail</t>
+  </si>
+  <si>
+    <t>Kite</t>
+  </si>
+  <si>
+    <t>Feathers</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>Hell_Roaring</t>
+  </si>
+  <si>
+    <t>Orangutan</t>
+  </si>
+  <si>
+    <t>Woodsy</t>
+  </si>
+  <si>
+    <t>Golden_winged_Warbler</t>
+  </si>
+  <si>
+    <t>Kid</t>
+  </si>
+  <si>
+    <t>Vanishing_Wilderness</t>
+  </si>
+  <si>
+    <t>Draggin</t>
+  </si>
+  <si>
+    <t>Busytown</t>
+  </si>
+  <si>
+    <t>Yowie</t>
+  </si>
+  <si>
+    <t>singer_Nicholas_Hexum</t>
+  </si>
+  <si>
+    <t>Nose</t>
+  </si>
+  <si>
+    <t>NBC_dramedy_Lipstick</t>
+  </si>
+  <si>
+    <t>Jungle_Swamp</t>
+  </si>
+  <si>
+    <t>Burro</t>
   </si>
 </sst>
 </file>
@@ -11293,10 +11350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AC216F-559C-4988-B135-E2C7D7D78959}">
-  <dimension ref="A1:A1684"/>
+  <dimension ref="A1:A1688"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A1653" workbookViewId="0">
-      <selection activeCell="A1684" sqref="A1684"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A1657" workbookViewId="0">
+      <selection activeCell="A1654" sqref="A1654:A1655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12529,16 +12586,6 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="246" spans="1:1">
-      <c r="A246" s="5" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1">
-      <c r="A247" s="6" t="s">
-        <v>2565</v>
-      </c>
-    </row>
     <row r="248" spans="1:1">
       <c r="A248" s="1" t="s">
         <v>48</v>
@@ -15934,16 +15981,6 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="927" spans="1:1">
-      <c r="A927" s="5" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="928" spans="1:1">
-      <c r="A928" s="6" t="s">
-        <v>2858</v>
-      </c>
-    </row>
     <row r="929" spans="1:1">
       <c r="A929" s="1" t="s">
         <v>179</v>
@@ -17419,11 +17456,6 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="1224" spans="1:1">
-      <c r="A1224" s="5" t="s">
-        <v>1594</v>
-      </c>
-    </row>
     <row r="1225" spans="1:1">
       <c r="A1225" s="1" t="s">
         <v>239</v>
@@ -19722,6 +19754,26 @@
     <row r="1684" spans="1:1" ht="15">
       <c r="A1684" s="7" t="s">
         <v>3452</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:1" ht="15">
+      <c r="A1685" s="7" t="s">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:1" ht="15">
+      <c r="A1686" s="7" t="s">
+        <v>3463</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:1" ht="15">
+      <c r="A1687" s="7" t="s">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:1" ht="15">
+      <c r="A1688" s="7" t="s">
+        <v>3470</v>
       </c>
     </row>
   </sheetData>
@@ -19735,10 +19787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BCBB88-EB20-4FE9-9853-5AEACCACF1D8}">
-  <dimension ref="A1:B1780"/>
+  <dimension ref="A1:B1800"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A1774" workbookViewId="0">
-      <selection activeCell="A1780" sqref="A1780"/>
+    <sheetView rightToLeft="1" topLeftCell="A1774" workbookViewId="0">
+      <selection activeCell="A1801" sqref="A1801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -28673,6 +28725,106 @@
         <v>3456</v>
       </c>
     </row>
+    <row r="1781" spans="1:1" ht="15">
+      <c r="A1781" s="7" t="s">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:1" ht="15">
+      <c r="A1782" s="7" t="s">
+        <v>3458</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:1" ht="15">
+      <c r="A1783" s="7" t="s">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:1" ht="15">
+      <c r="A1784" s="7" t="s">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:1" ht="15">
+      <c r="A1785" s="7" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:1" ht="15">
+      <c r="A1786" s="7" t="s">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:1" ht="15">
+      <c r="A1787" s="7" t="s">
+        <v>3466</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:1" ht="15">
+      <c r="A1788" s="7" t="s">
+        <v>3464</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:1" ht="15">
+      <c r="A1789" s="7" t="s">
+        <v>3467</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:1" ht="15">
+      <c r="A1790" s="7" t="s">
+        <v>3468</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:1" ht="15">
+      <c r="A1791" s="7" t="s">
+        <v>3469</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:1" ht="15">
+      <c r="A1792" s="7" t="s">
+        <v>3471</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:1" ht="15">
+      <c r="A1793" s="7" t="s">
+        <v>3472</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:1" ht="15">
+      <c r="A1794" s="7" t="s">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:1" ht="15">
+      <c r="A1795" s="7" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:1">
+      <c r="A1796" s="5" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:1">
+      <c r="A1797" s="6" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:1">
+      <c r="A1798" s="5" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:1">
+      <c r="A1799" s="6" t="s">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:1">
+      <c r="A1800" s="5" t="s">
+        <v>1594</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>